<commit_message>
Updated to Version 2
</commit_message>
<xml_diff>
--- a/Converting/converting_test_cases.xlsx
+++ b/Converting/converting_test_cases.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter\Documents\CPR101\GroupProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter\Documents\CPR101\GroupProject\Final Submission V1\2 Final Submission\CPR Group 1 Version 2\CPR Group 1 Version 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06E493D5-AF21-40AB-8ECC-6598F00643B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68EF2158-C5DF-48B0-B650-AB14955518E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1785" yWindow="1875" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4890" yWindow="2130" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCaseMatrix" sheetId="2" r:id="rId1"/>
@@ -121,7 +121,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B20" authorId="0" shapeId="0" xr:uid="{E121AF1F-0408-4713-A265-1FEF41AD73A9}">
+    <comment ref="B17" authorId="0" shapeId="0" xr:uid="{E121AF1F-0408-4713-A265-1FEF41AD73A9}">
       <text>
         <r>
           <rPr>
@@ -167,7 +167,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="55">
   <si>
     <t>Comments</t>
   </si>
@@ -245,9 +245,6 @@
     <t>void converting()</t>
   </si>
   <si>
-    <t>+ Enter a numeric string within the range of -2147483648 and 2147483647</t>
-  </si>
-  <si>
     <t>1234567890</t>
   </si>
   <si>
@@ -280,9 +277,6 @@
     <t>- After entering several negative tests (e.g., adding character strings, adding values outside of bounds -2147483648 and 2147483647), do normal inputs still produce correct outputs?</t>
   </si>
   <si>
-    <t>*** End of Converting Strings to int Demo ***</t>
-  </si>
-  <si>
     <t>Function will display the converted numerical string as an int on the screen, so long as the numerical string is within range.</t>
   </si>
   <si>
@@ -348,6 +342,57 @@
   </si>
   <si>
     <t>No safeguard has been placed to handle non-integer characters. See "Expected Result" for a possible error message that can be produced if the user enters a character that is not a number.</t>
+  </si>
+  <si>
+    <t>Converted number is 123
+Type the int numeric string (q - to quit):| Converted number is 99Type the int numeric string (q - to quit):|Converted number is 2147483647Converted number is 123
+Type the int numeric string (q - to quit):
+99
+Converted number is 99
+Type the int numeric string (q - to quit):
+q
+*** End of Converting Strings to int Demo ***
+Type the int numeric string (q - to quit):*** End of Converting Strings to int Demo ***</t>
+  </si>
+  <si>
+    <t>+ Enter a numeric string within the range of -2147483648 and 2147483647 (i.e., the size of a double).</t>
+  </si>
+  <si>
+    <t>2|123|8888</t>
+  </si>
+  <si>
+    <t>Converted number is 2.000000
+Type the double numeric string (q - to quit):
+123
+Converted number is 123.000000
+Type the double numeric string (q - to quit):
+8888
+Converted number is 8888.000000
+Type the double numeric string (q - to quit):</t>
+  </si>
+  <si>
+    <t>+ Enter various different strings within range within the range of 15^-307 and 15^-307 (i.e., the size of a double)</t>
+  </si>
+  <si>
+    <t>Function will display the converted numerical strings as a double on the screen, so long as the numerical string is within the range of a double.</t>
+  </si>
+  <si>
+    <t>Error! Enter numeric values only.
+Type the double numeric string (q - to quit):| Error! Enter numeric values only. Type the double numeric string (q - to quit):</t>
+  </si>
+  <si>
+    <t>Converted number is 0.000000
+Type the double numeric string (q - to quit):
+a55
+Converted number is 0.000000
+Type the double numeric string (q - to quit):</t>
+  </si>
+  <si>
+    <t>No safeguard has been placed to handle non-double characters. See "Expected Result" for a possible error message that can be produced if the user enters a character that is not a number.</t>
+  </si>
+  <si>
+    <t>Peter  Wan
+April 8, 2022</t>
   </si>
 </sst>
 </file>
@@ -1095,10 +1140,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1149,13 +1194,13 @@
         <v>7</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>2</v>
@@ -1170,22 +1215,22 @@
         <v>16</v>
       </c>
       <c r="B4" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="D4" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="33" t="s">
-        <v>19</v>
-      </c>
       <c r="G4" s="22" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H4" s="34"/>
       <c r="I4" s="35"/>
@@ -1195,22 +1240,22 @@
         <v>16</v>
       </c>
       <c r="B5" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>31</v>
-      </c>
       <c r="E5" s="18" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F5" s="33" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G5" s="22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H5" s="34"/>
       <c r="I5" s="35"/>
@@ -1220,47 +1265,47 @@
         <v>16</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F6" s="33" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G6" s="22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H6" s="34"/>
       <c r="I6" s="35"/>
     </row>
-    <row r="7" spans="1:9" ht="102" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="19" t="s">
-        <v>39</v>
-      </c>
       <c r="D7" s="19" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F7" s="33" t="s">
         <v>5</v>
       </c>
       <c r="G7" s="22" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H7" s="34"/>
       <c r="I7" s="35"/>
@@ -1270,47 +1315,47 @@
         <v>16</v>
       </c>
       <c r="B8" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="20" t="s">
         <v>41</v>
-      </c>
-      <c r="C8" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="D8" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="E8" s="20" t="s">
-        <v>43</v>
       </c>
       <c r="F8" s="33" t="s">
         <v>5</v>
       </c>
       <c r="G8" s="22" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H8" s="34"/>
       <c r="I8" s="35"/>
     </row>
-    <row r="9" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="242.25" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="22" t="s">
         <v>32</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="G9" s="22" t="s">
-        <v>34</v>
       </c>
       <c r="H9" s="34"/>
       <c r="I9" s="35"/>
@@ -1338,7 +1383,7 @@
         <v>9</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>10</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="14" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1365,57 +1410,118 @@
       </c>
       <c r="I12" s="15"/>
     </row>
-    <row r="13" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A13" s="36"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="25"/>
+    <row r="13" spans="1:9" ht="165.75" x14ac:dyDescent="0.2">
+      <c r="A13" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" s="22" t="s">
+        <v>50</v>
+      </c>
       <c r="I13" s="35"/>
     </row>
-    <row r="14" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A14" s="36"/>
-      <c r="B14" s="23"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="25"/>
-      <c r="I14" s="35"/>
-    </row>
-    <row r="15" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A15" s="36"/>
-      <c r="B15" s="23"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="25"/>
-      <c r="I15" s="35"/>
-    </row>
-    <row r="16" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A16" s="36"/>
-      <c r="B16" s="23"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="25"/>
-      <c r="I16" s="35"/>
-    </row>
-    <row r="17" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A17" s="36"/>
-      <c r="B17" s="23"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="33"/>
-      <c r="G17" s="25"/>
-      <c r="I17" s="37"/>
-    </row>
-    <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A14" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="F14" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="G14" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="I14" s="37"/>
+    </row>
+    <row r="15" spans="1:9" ht="243" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="I15" s="37"/>
+    </row>
+    <row r="16" spans="1:9" s="14" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="14" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="I17" s="15"/>
+    </row>
+    <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="36"/>
       <c r="B18" s="23"/>
       <c r="C18" s="21"/>
@@ -1425,44 +1531,25 @@
       <c r="G18" s="25"/>
       <c r="I18" s="37"/>
     </row>
-    <row r="19" spans="1:9" s="14" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G19" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" s="14" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F20" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="G20" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="I20" s="15"/>
+    <row r="19" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A19" s="36"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="25"/>
+      <c r="I19" s="37"/>
+    </row>
+    <row r="20" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A20" s="36"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="33"/>
+      <c r="G20" s="25"/>
+      <c r="I20" s="37"/>
     </row>
     <row r="21" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" s="36"/>
@@ -1478,8 +1565,8 @@
       <c r="A22" s="36"/>
       <c r="B22" s="23"/>
       <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="24"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="25"/>
       <c r="F22" s="33"/>
       <c r="G22" s="25"/>
       <c r="I22" s="37"/>
@@ -1488,8 +1575,8 @@
       <c r="A23" s="36"/>
       <c r="B23" s="23"/>
       <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="24"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="25"/>
       <c r="F23" s="33"/>
       <c r="G23" s="25"/>
       <c r="I23" s="37"/>
@@ -1498,8 +1585,8 @@
       <c r="A24" s="36"/>
       <c r="B24" s="23"/>
       <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="24"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="25"/>
       <c r="F24" s="33"/>
       <c r="G24" s="25"/>
       <c r="I24" s="37"/>
@@ -1514,51 +1601,21 @@
       <c r="G25" s="25"/>
       <c r="I25" s="37"/>
     </row>
-    <row r="26" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A26" s="36"/>
-      <c r="B26" s="23"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="33"/>
-      <c r="G26" s="25"/>
-      <c r="I26" s="37"/>
-    </row>
-    <row r="27" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A27" s="36"/>
-      <c r="B27" s="23"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="25"/>
-      <c r="I27" s="37"/>
-    </row>
-    <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A28" s="36"/>
-      <c r="B28" s="23"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="33"/>
-      <c r="G28" s="25"/>
-      <c r="I28" s="37"/>
-    </row>
-    <row r="29" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="38"/>
-      <c r="B29" s="27"/>
-      <c r="C29" s="28"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="30"/>
+    <row r="26" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="38"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="39"/>
+      <c r="G26" s="30"/>
     </row>
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="3">
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A11:E11"/>
-    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="A16:E16"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1801,13 +1858,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCBC8B3B-5513-4AE1-AEAC-83542AFBEF22}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4AD3CEDD-CAA5-4023-AA87-9C98C4C7D9BE}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91299321-BC00-4DD7-8BA4-D70BF65B0812}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DB0944A-AA04-420C-A5D4-08FC71285F3A}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C77A9B5-E09B-4662-9B9D-CA35BE179084}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57F3BDFA-F5F7-499B-B2CC-6B5F16016208}"/>
 </file>
</xml_diff>